<commit_message>
Atualizando Requisitos e Casos de Uso
</commit_message>
<xml_diff>
--- a/Requisitos Textion.xlsx
+++ b/Requisitos Textion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\textion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>RE Nº</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Leitor e Autor</t>
   </si>
   <si>
-    <t>Permitir cadastro de autor ou leitor</t>
-  </si>
-  <si>
     <t>Permitir que um leitor torne-se autor</t>
   </si>
   <si>
@@ -53,12 +50,6 @@
     <t xml:space="preserve">Permitir sugestões de temas e autores para leitura na home </t>
   </si>
   <si>
-    <t>Leitor, Autor e Usuário</t>
-  </si>
-  <si>
-    <t>Permitir que o leitor faça comentários sobre os textos</t>
-  </si>
-  <si>
     <t>Leitor</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>Permitir avaliação das livrarias indicadas</t>
   </si>
   <si>
-    <t>Cadastrar Leitor e Autor</t>
-  </si>
-  <si>
     <t>Sugerir temas e autores</t>
   </si>
   <si>
@@ -149,7 +137,88 @@
     <t>Publicar livro</t>
   </si>
   <si>
-    <t xml:space="preserve">Alterar conta </t>
+    <t>Permitir que leitor leia o texto</t>
+  </si>
+  <si>
+    <t>Ler texto</t>
+  </si>
+  <si>
+    <t>UC01</t>
+  </si>
+  <si>
+    <t>UC02</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC04</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
+    <t>UC06</t>
+  </si>
+  <si>
+    <t>UC07</t>
+  </si>
+  <si>
+    <t>UC08</t>
+  </si>
+  <si>
+    <t>UC09</t>
+  </si>
+  <si>
+    <t>UC10</t>
+  </si>
+  <si>
+    <t>UC11</t>
+  </si>
+  <si>
+    <t>UC12</t>
+  </si>
+  <si>
+    <t>UC13</t>
+  </si>
+  <si>
+    <t>UC14</t>
+  </si>
+  <si>
+    <t>UC15</t>
+  </si>
+  <si>
+    <t>UC16</t>
+  </si>
+  <si>
+    <t>UC17</t>
+  </si>
+  <si>
+    <t>Permitir cadastro de  leitor</t>
+  </si>
+  <si>
+    <t>Leitor, Autor e Visitante</t>
+  </si>
+  <si>
+    <t>Permitir cadastro de  autor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastrar Leitor </t>
+  </si>
+  <si>
+    <t>Cadastrar Autor</t>
+  </si>
+  <si>
+    <t>UC18</t>
+  </si>
+  <si>
+    <t>Permitir que faça comentários sobre os textos</t>
+  </si>
+  <si>
+    <t>Leitor, Visitante e Autor</t>
+  </si>
+  <si>
+    <t>Tornar-se Autor</t>
   </si>
 </sst>
 </file>
@@ -173,12 +242,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,10 +268,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,20 +557,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.375" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,228 +584,315 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>